<commit_message>
Fiz o docstrings de todas as funções do projeto
</commit_message>
<xml_diff>
--- a/Produtos.xlsx
+++ b/Produtos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,20 +463,58 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Arroz</t>
+          <t>Arroz 5kg</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2247</v>
+        <v>2254</v>
       </c>
       <c r="C2" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D2" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E2" t="n">
-        <v>26</v>
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Feijão COMBRASIL 1kg</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1501</v>
+      </c>
+      <c r="C3" t="n">
+        <v>17.8</v>
+      </c>
+      <c r="D3" t="n">
+        <v>49</v>
+      </c>
+      <c r="E3" t="n">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Macarrão Maximus</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>2571</v>
+      </c>
+      <c r="C4" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="D4" t="n">
+        <v>23</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>